<commit_message>
Fix bug related to events with the same ID, add CM groups to course info
</commit_message>
<xml_diff>
--- a/data/DEUST.xlsx
+++ b/data/DEUST.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/SSDS/enseignement/UFR STAPS/Direction/Outils/celcatreport/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412FFF15-0D7A-8640-B9C5-166F57D51935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D9EC19-1227-504E-9ECD-FEE85290D88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19580" xr2:uid="{154AE90F-D41B-8B49-BA91-D855BEB6F170}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>Code Apogée</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Porter secours à tout public en milieu aquatique - UE SSMA C3</t>
+  </si>
+  <si>
+    <t>Groupes CM</t>
   </si>
 </sst>
 </file>
@@ -620,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D425352-B3D2-6642-82B3-EC9BD51219AA}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,7 +637,7 @@
     <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -651,19 +654,22 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -680,19 +686,22 @@
         <v>0</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>30</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -709,19 +718,22 @@
         <v>0</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>48</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -738,19 +750,22 @@
         <v>0</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>29</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -767,19 +782,22 @@
         <v>0</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>30</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -796,19 +814,22 @@
         <v>0</v>
       </c>
       <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>50</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -825,19 +846,22 @@
         <v>0</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>7</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -854,19 +878,22 @@
         <v>0</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>11</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -883,19 +910,22 @@
         <v>0</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>17</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
       <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>12</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -912,19 +942,22 @@
         <v>0</v>
       </c>
       <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>11</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
       <c r="H10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -941,19 +974,22 @@
         <v>0</v>
       </c>
       <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>20</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
       <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>15</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -970,19 +1006,22 @@
         <v>0</v>
       </c>
       <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>45</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -999,19 +1038,22 @@
         <v>0</v>
       </c>
       <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
         <v>35</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1028,19 +1070,22 @@
         <v>6</v>
       </c>
       <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>35</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1057,19 +1102,22 @@
         <v>0</v>
       </c>
       <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>50</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1086,19 +1134,22 @@
         <v>0</v>
       </c>
       <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
         <v>10</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1115,19 +1166,22 @@
         <v>0</v>
       </c>
       <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
         <v>13</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
       <c r="H17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1144,19 +1198,22 @@
         <v>0</v>
       </c>
       <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
         <v>15</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
       <c r="H18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1173,19 +1230,22 @@
         <v>0</v>
       </c>
       <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
         <v>40</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1202,19 +1262,22 @@
         <v>0</v>
       </c>
       <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
         <v>39</v>
       </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1231,19 +1294,22 @@
         <v>0</v>
       </c>
       <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
         <v>40</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1260,19 +1326,22 @@
         <v>0</v>
       </c>
       <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
         <v>30</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1289,19 +1358,22 @@
         <v>0</v>
       </c>
       <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
         <v>50</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1318,19 +1390,22 @@
         <v>0</v>
       </c>
       <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
         <v>23</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
       <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
         <v>15</v>
       </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1347,19 +1422,22 @@
         <v>0</v>
       </c>
       <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
         <v>12</v>
       </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1376,19 +1454,22 @@
         <v>0</v>
       </c>
       <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
         <v>20</v>
       </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
       <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
         <v>10</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1405,19 +1486,22 @@
         <v>0</v>
       </c>
       <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
         <v>20</v>
       </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
       <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
         <v>10</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1434,19 +1518,22 @@
         <v>0</v>
       </c>
       <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
         <v>30</v>
       </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1463,19 +1550,22 @@
         <v>6</v>
       </c>
       <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
         <v>25</v>
       </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1492,19 +1582,22 @@
         <v>0</v>
       </c>
       <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <v>50</v>
       </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
       <c r="H30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -1521,19 +1614,22 @@
         <v>0</v>
       </c>
       <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
         <v>12</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
       <c r="H31">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -1550,19 +1646,22 @@
         <v>0</v>
       </c>
       <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
         <v>16</v>
       </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
       <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
         <v>22</v>
       </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1579,20 +1678,23 @@
         <v>0</v>
       </c>
       <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
         <v>9</v>
       </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
       <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
         <v>15</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I41">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J41">
     <sortCondition ref="B2:B41"/>
     <sortCondition ref="A2:A41"/>
   </sortState>

</xml_diff>